<commit_message>
added pivoted table and to do list
</commit_message>
<xml_diff>
--- a/atlanta-census.xlsx
+++ b/atlanta-census.xlsx
@@ -469,25 +469,17 @@
           <t>Total:</t>
         </is>
       </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>463,875</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>472,506</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>486,299</t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>498,073</t>
-        </is>
+      <c r="C2" t="n">
+        <v>463875</v>
+      </c>
+      <c r="D2" t="n">
+        <v>472506</v>
+      </c>
+      <c r="E2" t="n">
+        <v>486299</v>
+      </c>
+      <c r="F2" t="n">
+        <v>498073</v>
       </c>
     </row>
     <row r="3">
@@ -499,25 +491,17 @@
           <t xml:space="preserve">    Not Hispanic or Latino:</t>
         </is>
       </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>445,222</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>449,408</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>465,421</t>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>475,094</t>
-        </is>
+      <c r="C3" t="n">
+        <v>445222</v>
+      </c>
+      <c r="D3" t="n">
+        <v>449408</v>
+      </c>
+      <c r="E3" t="n">
+        <v>465421</v>
+      </c>
+      <c r="F3" t="n">
+        <v>475094</v>
       </c>
     </row>
     <row r="4">
@@ -529,25 +513,17 @@
           <t xml:space="preserve">        White alone</t>
         </is>
       </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>176,998</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>178,077</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>179,296</t>
-        </is>
-      </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>189,230</t>
-        </is>
+      <c r="C4" t="n">
+        <v>176998</v>
+      </c>
+      <c r="D4" t="n">
+        <v>178077</v>
+      </c>
+      <c r="E4" t="n">
+        <v>179296</v>
+      </c>
+      <c r="F4" t="n">
+        <v>189230</v>
       </c>
     </row>
     <row r="5">
@@ -559,25 +535,17 @@
           <t xml:space="preserve">        Black or African American alone</t>
         </is>
       </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>239,159</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>237,590</t>
-        </is>
-      </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>253,556</t>
-        </is>
-      </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>252,493</t>
-        </is>
+      <c r="C5" t="n">
+        <v>239159</v>
+      </c>
+      <c r="D5" t="n">
+        <v>237590</v>
+      </c>
+      <c r="E5" t="n">
+        <v>253556</v>
+      </c>
+      <c r="F5" t="n">
+        <v>252493</v>
       </c>
     </row>
     <row r="6">
@@ -589,25 +557,17 @@
           <t xml:space="preserve">        American Indian and Alaska Native alone</t>
         </is>
       </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>652</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>951</t>
-        </is>
-      </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>374</t>
-        </is>
-      </c>
-      <c r="F6" t="inlineStr">
-        <is>
-          <t>495</t>
-        </is>
+      <c r="C6" t="n">
+        <v>652</v>
+      </c>
+      <c r="D6" t="n">
+        <v>951</v>
+      </c>
+      <c r="E6" t="n">
+        <v>374</v>
+      </c>
+      <c r="F6" t="n">
+        <v>495</v>
       </c>
     </row>
     <row r="7">
@@ -619,25 +579,17 @@
           <t xml:space="preserve">        Asian alone</t>
         </is>
       </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>20,335</t>
-        </is>
-      </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>20,253</t>
-        </is>
-      </c>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t>19,551</t>
-        </is>
-      </c>
-      <c r="F7" t="inlineStr">
-        <is>
-          <t>19,875</t>
-        </is>
+      <c r="C7" t="n">
+        <v>20335</v>
+      </c>
+      <c r="D7" t="n">
+        <v>20253</v>
+      </c>
+      <c r="E7" t="n">
+        <v>19551</v>
+      </c>
+      <c r="F7" t="n">
+        <v>19875</v>
       </c>
     </row>
     <row r="8">
@@ -649,25 +601,17 @@
           <t xml:space="preserve">        Native Hawaiian and Other Pacific Islander alone</t>
         </is>
       </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>147</t>
-        </is>
-      </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>170</t>
-        </is>
-      </c>
-      <c r="E8" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="F8" t="inlineStr">
-        <is>
-          <t>142</t>
-        </is>
+      <c r="C8" t="n">
+        <v>147</v>
+      </c>
+      <c r="D8" t="n">
+        <v>170</v>
+      </c>
+      <c r="E8" t="n">
+        <v>0</v>
+      </c>
+      <c r="F8" t="n">
+        <v>142</v>
       </c>
     </row>
     <row r="9">
@@ -679,25 +623,17 @@
           <t xml:space="preserve">        Some other race alone</t>
         </is>
       </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>265</t>
-        </is>
-      </c>
-      <c r="D9" t="inlineStr">
-        <is>
-          <t>481</t>
-        </is>
-      </c>
-      <c r="E9" t="inlineStr">
-        <is>
-          <t>2,129</t>
-        </is>
-      </c>
-      <c r="F9" t="inlineStr">
-        <is>
-          <t>1,324</t>
-        </is>
+      <c r="C9" t="n">
+        <v>265</v>
+      </c>
+      <c r="D9" t="n">
+        <v>481</v>
+      </c>
+      <c r="E9" t="n">
+        <v>2129</v>
+      </c>
+      <c r="F9" t="n">
+        <v>1324</v>
       </c>
     </row>
     <row r="10">
@@ -709,25 +645,17 @@
           <t xml:space="preserve">        Two or more races:</t>
         </is>
       </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>7,666</t>
-        </is>
-      </c>
-      <c r="D10" t="inlineStr">
-        <is>
-          <t>11,886</t>
-        </is>
-      </c>
-      <c r="E10" t="inlineStr">
-        <is>
-          <t>10,515</t>
-        </is>
-      </c>
-      <c r="F10" t="inlineStr">
-        <is>
-          <t>11,535</t>
-        </is>
+      <c r="C10" t="n">
+        <v>7666</v>
+      </c>
+      <c r="D10" t="n">
+        <v>11886</v>
+      </c>
+      <c r="E10" t="n">
+        <v>10515</v>
+      </c>
+      <c r="F10" t="n">
+        <v>11535</v>
       </c>
     </row>
     <row r="11">
@@ -739,25 +667,17 @@
           <t xml:space="preserve">            Two races including Some other race</t>
         </is>
       </c>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t>405</t>
-        </is>
-      </c>
-      <c r="D11" t="inlineStr">
-        <is>
-          <t>1,236</t>
-        </is>
-      </c>
-      <c r="E11" t="inlineStr">
-        <is>
-          <t>144</t>
-        </is>
-      </c>
-      <c r="F11" t="inlineStr">
-        <is>
-          <t>471</t>
-        </is>
+      <c r="C11" t="n">
+        <v>405</v>
+      </c>
+      <c r="D11" t="n">
+        <v>1236</v>
+      </c>
+      <c r="E11" t="n">
+        <v>144</v>
+      </c>
+      <c r="F11" t="n">
+        <v>471</v>
       </c>
     </row>
     <row r="12">
@@ -769,25 +689,17 @@
           <t xml:space="preserve">            Two races excluding Some other race, and three or more races</t>
         </is>
       </c>
-      <c r="C12" t="inlineStr">
-        <is>
-          <t>7,261</t>
-        </is>
-      </c>
-      <c r="D12" t="inlineStr">
-        <is>
-          <t>10,650</t>
-        </is>
-      </c>
-      <c r="E12" t="inlineStr">
-        <is>
-          <t>10,371</t>
-        </is>
-      </c>
-      <c r="F12" t="inlineStr">
-        <is>
-          <t>11,064</t>
-        </is>
+      <c r="C12" t="n">
+        <v>7261</v>
+      </c>
+      <c r="D12" t="n">
+        <v>10650</v>
+      </c>
+      <c r="E12" t="n">
+        <v>10371</v>
+      </c>
+      <c r="F12" t="n">
+        <v>11064</v>
       </c>
     </row>
     <row r="13">
@@ -799,25 +711,17 @@
           <t xml:space="preserve">    Hispanic or Latino:</t>
         </is>
       </c>
-      <c r="C13" t="inlineStr">
-        <is>
-          <t>18,653</t>
-        </is>
-      </c>
-      <c r="D13" t="inlineStr">
-        <is>
-          <t>23,098</t>
-        </is>
-      </c>
-      <c r="E13" t="inlineStr">
-        <is>
-          <t>20,878</t>
-        </is>
-      </c>
-      <c r="F13" t="inlineStr">
-        <is>
-          <t>22,979</t>
-        </is>
+      <c r="C13" t="n">
+        <v>18653</v>
+      </c>
+      <c r="D13" t="n">
+        <v>23098</v>
+      </c>
+      <c r="E13" t="n">
+        <v>20878</v>
+      </c>
+      <c r="F13" t="n">
+        <v>22979</v>
       </c>
     </row>
     <row r="14">
@@ -829,25 +733,17 @@
           <t xml:space="preserve">        White alone</t>
         </is>
       </c>
-      <c r="C14" t="inlineStr">
-        <is>
-          <t>12,155</t>
-        </is>
-      </c>
-      <c r="D14" t="inlineStr">
-        <is>
-          <t>12,815</t>
-        </is>
-      </c>
-      <c r="E14" t="inlineStr">
-        <is>
-          <t>11,119</t>
-        </is>
-      </c>
-      <c r="F14" t="inlineStr">
-        <is>
-          <t>14,285</t>
-        </is>
+      <c r="C14" t="n">
+        <v>12155</v>
+      </c>
+      <c r="D14" t="n">
+        <v>12815</v>
+      </c>
+      <c r="E14" t="n">
+        <v>11119</v>
+      </c>
+      <c r="F14" t="n">
+        <v>14285</v>
       </c>
     </row>
     <row r="15">
@@ -859,25 +755,17 @@
           <t xml:space="preserve">        Black or African American alone</t>
         </is>
       </c>
-      <c r="C15" t="inlineStr">
-        <is>
-          <t>1,440</t>
-        </is>
-      </c>
-      <c r="D15" t="inlineStr">
-        <is>
-          <t>2,612</t>
-        </is>
-      </c>
-      <c r="E15" t="inlineStr">
-        <is>
-          <t>3,332</t>
-        </is>
-      </c>
-      <c r="F15" t="inlineStr">
-        <is>
-          <t>1,277</t>
-        </is>
+      <c r="C15" t="n">
+        <v>1440</v>
+      </c>
+      <c r="D15" t="n">
+        <v>2612</v>
+      </c>
+      <c r="E15" t="n">
+        <v>3332</v>
+      </c>
+      <c r="F15" t="n">
+        <v>1277</v>
       </c>
     </row>
     <row r="16">
@@ -889,25 +777,17 @@
           <t xml:space="preserve">        American Indian and Alaska Native alone</t>
         </is>
       </c>
-      <c r="C16" t="inlineStr">
-        <is>
-          <t>651</t>
-        </is>
-      </c>
-      <c r="D16" t="inlineStr">
-        <is>
-          <t>1,944</t>
-        </is>
-      </c>
-      <c r="E16" t="inlineStr">
-        <is>
-          <t>330</t>
-        </is>
-      </c>
-      <c r="F16" t="inlineStr">
-        <is>
-          <t>323</t>
-        </is>
+      <c r="C16" t="n">
+        <v>651</v>
+      </c>
+      <c r="D16" t="n">
+        <v>1944</v>
+      </c>
+      <c r="E16" t="n">
+        <v>330</v>
+      </c>
+      <c r="F16" t="n">
+        <v>323</v>
       </c>
     </row>
     <row r="17">
@@ -919,25 +799,17 @@
           <t xml:space="preserve">        Asian alone</t>
         </is>
       </c>
-      <c r="C17" t="inlineStr">
-        <is>
-          <t>81</t>
-        </is>
-      </c>
-      <c r="D17" t="inlineStr">
-        <is>
-          <t>197</t>
-        </is>
-      </c>
-      <c r="E17" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="F17" t="inlineStr">
-        <is>
-          <t>144</t>
-        </is>
+      <c r="C17" t="n">
+        <v>81</v>
+      </c>
+      <c r="D17" t="n">
+        <v>197</v>
+      </c>
+      <c r="E17" t="n">
+        <v>0</v>
+      </c>
+      <c r="F17" t="n">
+        <v>144</v>
       </c>
     </row>
     <row r="18">
@@ -949,25 +821,17 @@
           <t xml:space="preserve">        Native Hawaiian and Other Pacific Islander alone</t>
         </is>
       </c>
-      <c r="C18" t="inlineStr">
-        <is>
-          <t>316</t>
-        </is>
-      </c>
-      <c r="D18" t="inlineStr">
-        <is>
-          <t>39</t>
-        </is>
-      </c>
-      <c r="E18" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="F18" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+      <c r="C18" t="n">
+        <v>316</v>
+      </c>
+      <c r="D18" t="n">
+        <v>39</v>
+      </c>
+      <c r="E18" t="n">
+        <v>0</v>
+      </c>
+      <c r="F18" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="19">
@@ -979,25 +843,17 @@
           <t xml:space="preserve">        Some other race alone</t>
         </is>
       </c>
-      <c r="C19" t="inlineStr">
-        <is>
-          <t>2,282</t>
-        </is>
-      </c>
-      <c r="D19" t="inlineStr">
-        <is>
-          <t>3,482</t>
-        </is>
-      </c>
-      <c r="E19" t="inlineStr">
-        <is>
-          <t>4,409</t>
-        </is>
-      </c>
-      <c r="F19" t="inlineStr">
-        <is>
-          <t>5,214</t>
-        </is>
+      <c r="C19" t="n">
+        <v>2282</v>
+      </c>
+      <c r="D19" t="n">
+        <v>3482</v>
+      </c>
+      <c r="E19" t="n">
+        <v>4409</v>
+      </c>
+      <c r="F19" t="n">
+        <v>5214</v>
       </c>
     </row>
     <row r="20">
@@ -1009,25 +865,17 @@
           <t xml:space="preserve">        Two or more races:</t>
         </is>
       </c>
-      <c r="C20" t="inlineStr">
-        <is>
-          <t>1,728</t>
-        </is>
-      </c>
-      <c r="D20" t="inlineStr">
-        <is>
-          <t>2,009</t>
-        </is>
-      </c>
-      <c r="E20" t="inlineStr">
-        <is>
-          <t>1,688</t>
-        </is>
-      </c>
-      <c r="F20" t="inlineStr">
-        <is>
-          <t>1,736</t>
-        </is>
+      <c r="C20" t="n">
+        <v>1728</v>
+      </c>
+      <c r="D20" t="n">
+        <v>2009</v>
+      </c>
+      <c r="E20" t="n">
+        <v>1688</v>
+      </c>
+      <c r="F20" t="n">
+        <v>1736</v>
       </c>
     </row>
     <row r="21">
@@ -1039,25 +887,17 @@
           <t xml:space="preserve">            Two races including Some other race</t>
         </is>
       </c>
-      <c r="C21" t="inlineStr">
-        <is>
-          <t>529</t>
-        </is>
-      </c>
-      <c r="D21" t="inlineStr">
-        <is>
-          <t>578</t>
-        </is>
-      </c>
-      <c r="E21" t="inlineStr">
-        <is>
-          <t>766</t>
-        </is>
-      </c>
-      <c r="F21" t="inlineStr">
-        <is>
-          <t>571</t>
-        </is>
+      <c r="C21" t="n">
+        <v>529</v>
+      </c>
+      <c r="D21" t="n">
+        <v>578</v>
+      </c>
+      <c r="E21" t="n">
+        <v>766</v>
+      </c>
+      <c r="F21" t="n">
+        <v>571</v>
       </c>
     </row>
     <row r="22">
@@ -1069,25 +909,17 @@
           <t xml:space="preserve">            Two races excluding Some other race, and three or more races</t>
         </is>
       </c>
-      <c r="C22" t="inlineStr">
-        <is>
-          <t>1,199</t>
-        </is>
-      </c>
-      <c r="D22" t="inlineStr">
-        <is>
-          <t>1,431</t>
-        </is>
-      </c>
-      <c r="E22" t="inlineStr">
-        <is>
-          <t>922</t>
-        </is>
-      </c>
-      <c r="F22" t="inlineStr">
-        <is>
-          <t>1,165</t>
-        </is>
+      <c r="C22" t="n">
+        <v>1199</v>
+      </c>
+      <c r="D22" t="n">
+        <v>1431</v>
+      </c>
+      <c r="E22" t="n">
+        <v>922</v>
+      </c>
+      <c r="F22" t="n">
+        <v>1165</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added Yearly Average Sheet to 'avocado_years.xlsx'
</commit_message>
<xml_diff>
--- a/atlanta-census.xlsx
+++ b/atlanta-census.xlsx
@@ -1,37 +1,123 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <workbookPr/>
-  <workbookProtection/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="2015-2018" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="2015-2018" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
+  <si>
+    <t>group</t>
+  </si>
+  <si>
+    <t>2015</t>
+  </si>
+  <si>
+    <t>2016</t>
+  </si>
+  <si>
+    <t>2017</t>
+  </si>
+  <si>
+    <t>2018</t>
+  </si>
+  <si>
+    <t>Total:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Not Hispanic or Latino:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        White alone</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        Black or African American alone</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        American Indian and Alaska Native alone</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        Asian alone</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        Native Hawaiian and Other Pacific Islander alone</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        Some other race alone</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        Two or more races:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">            Two races including Some other race</t>
+  </si>
+  <si>
+    <t xml:space="preserve">            Two races excluding Some other race, and three or more races</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Hispanic or Latino:</t>
+  </si>
+  <si>
+    <t>h_white_alone</t>
+  </si>
+  <si>
+    <t>h_black_or_african-american</t>
+  </si>
+  <si>
+    <t>h_american_indian_and_alaska_native</t>
+  </si>
+  <si>
+    <t>h_asian</t>
+  </si>
+  <si>
+    <t>h_native_hawaiian_pacific_islander</t>
+  </si>
+  <si>
+    <t>h_other</t>
+  </si>
+  <si>
+    <t>h_two_or_more_races_total</t>
+  </si>
+  <si>
+    <t>h_two_races_including_some_other_race</t>
+  </si>
+  <si>
+    <t>h_two_races_excluing_some_other_race</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
   <fonts count="2">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <color theme="1"/>
-      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b val="1"/>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill/>
+      <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -46,93 +132,35 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008000"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00808000"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="009999FF"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00FFFFCC"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00660066"/>
-      <rgbColor rgb="00FF8080"/>
-      <rgbColor rgb="000066CC"/>
-      <rgbColor rgb="00CCCCFF"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
-    </indexedColors>
-  </colors>
 </styleSheet>
 </file>
 
@@ -420,509 +448,451 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1">
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>group</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>2015</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>2016</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>2017</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>2018</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="1" t="n">
+    <row r="1" spans="1:6">
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>Total:</t>
-        </is>
-      </c>
-      <c r="C2" t="n">
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" s="1">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2">
         <v>463875</v>
       </c>
-      <c r="D2" t="n">
+      <c r="D2">
         <v>472506</v>
       </c>
-      <c r="E2" t="n">
+      <c r="E2">
         <v>486299</v>
       </c>
-      <c r="F2" t="n">
+      <c r="F2">
         <v>498073</v>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" s="1" t="n">
+    <row r="3" spans="1:6">
+      <c r="A3" s="1">
         <v>1</v>
       </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t xml:space="preserve">    Not Hispanic or Latino:</t>
-        </is>
-      </c>
-      <c r="C3" t="n">
+      <c r="B3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3">
         <v>445222</v>
       </c>
-      <c r="D3" t="n">
+      <c r="D3">
         <v>449408</v>
       </c>
-      <c r="E3" t="n">
+      <c r="E3">
         <v>465421</v>
       </c>
-      <c r="F3" t="n">
+      <c r="F3">
         <v>475094</v>
       </c>
     </row>
-    <row r="4">
-      <c r="A4" s="1" t="n">
+    <row r="4" spans="1:6">
+      <c r="A4" s="1">
         <v>2</v>
       </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t xml:space="preserve">        White alone</t>
-        </is>
-      </c>
-      <c r="C4" t="n">
+      <c r="B4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4">
         <v>176998</v>
       </c>
-      <c r="D4" t="n">
+      <c r="D4">
         <v>178077</v>
       </c>
-      <c r="E4" t="n">
+      <c r="E4">
         <v>179296</v>
       </c>
-      <c r="F4" t="n">
+      <c r="F4">
         <v>189230</v>
       </c>
     </row>
-    <row r="5">
-      <c r="A5" s="1" t="n">
+    <row r="5" spans="1:6">
+      <c r="A5" s="1">
         <v>3</v>
       </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t xml:space="preserve">        Black or African American alone</t>
-        </is>
-      </c>
-      <c r="C5" t="n">
+      <c r="B5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5">
         <v>239159</v>
       </c>
-      <c r="D5" t="n">
+      <c r="D5">
         <v>237590</v>
       </c>
-      <c r="E5" t="n">
+      <c r="E5">
         <v>253556</v>
       </c>
-      <c r="F5" t="n">
+      <c r="F5">
         <v>252493</v>
       </c>
     </row>
-    <row r="6">
-      <c r="A6" s="1" t="n">
+    <row r="6" spans="1:6">
+      <c r="A6" s="1">
         <v>4</v>
       </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t xml:space="preserve">        American Indian and Alaska Native alone</t>
-        </is>
-      </c>
-      <c r="C6" t="n">
+      <c r="B6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6">
         <v>652</v>
       </c>
-      <c r="D6" t="n">
+      <c r="D6">
         <v>951</v>
       </c>
-      <c r="E6" t="n">
+      <c r="E6">
         <v>374</v>
       </c>
-      <c r="F6" t="n">
+      <c r="F6">
         <v>495</v>
       </c>
     </row>
-    <row r="7">
-      <c r="A7" s="1" t="n">
+    <row r="7" spans="1:6">
+      <c r="A7" s="1">
         <v>5</v>
       </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t xml:space="preserve">        Asian alone</t>
-        </is>
-      </c>
-      <c r="C7" t="n">
+      <c r="B7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7">
         <v>20335</v>
       </c>
-      <c r="D7" t="n">
+      <c r="D7">
         <v>20253</v>
       </c>
-      <c r="E7" t="n">
+      <c r="E7">
         <v>19551</v>
       </c>
-      <c r="F7" t="n">
+      <c r="F7">
         <v>19875</v>
       </c>
     </row>
-    <row r="8">
-      <c r="A8" s="1" t="n">
+    <row r="8" spans="1:6">
+      <c r="A8" s="1">
         <v>6</v>
       </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t xml:space="preserve">        Native Hawaiian and Other Pacific Islander alone</t>
-        </is>
-      </c>
-      <c r="C8" t="n">
+      <c r="B8" t="s">
+        <v>11</v>
+      </c>
+      <c r="C8">
         <v>147</v>
       </c>
-      <c r="D8" t="n">
+      <c r="D8">
         <v>170</v>
       </c>
-      <c r="E8" t="n">
+      <c r="E8">
         <v>0</v>
       </c>
-      <c r="F8" t="n">
+      <c r="F8">
         <v>142</v>
       </c>
     </row>
-    <row r="9">
-      <c r="A9" s="1" t="n">
+    <row r="9" spans="1:6">
+      <c r="A9" s="1">
         <v>7</v>
       </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t xml:space="preserve">        Some other race alone</t>
-        </is>
-      </c>
-      <c r="C9" t="n">
+      <c r="B9" t="s">
+        <v>12</v>
+      </c>
+      <c r="C9">
         <v>265</v>
       </c>
-      <c r="D9" t="n">
+      <c r="D9">
         <v>481</v>
       </c>
-      <c r="E9" t="n">
+      <c r="E9">
         <v>2129</v>
       </c>
-      <c r="F9" t="n">
+      <c r="F9">
         <v>1324</v>
       </c>
     </row>
-    <row r="10">
-      <c r="A10" s="1" t="n">
+    <row r="10" spans="1:6">
+      <c r="A10" s="1">
         <v>8</v>
       </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t xml:space="preserve">        Two or more races:</t>
-        </is>
-      </c>
-      <c r="C10" t="n">
+      <c r="B10" t="s">
+        <v>13</v>
+      </c>
+      <c r="C10">
         <v>7666</v>
       </c>
-      <c r="D10" t="n">
+      <c r="D10">
         <v>11886</v>
       </c>
-      <c r="E10" t="n">
+      <c r="E10">
         <v>10515</v>
       </c>
-      <c r="F10" t="n">
+      <c r="F10">
         <v>11535</v>
       </c>
     </row>
-    <row r="11">
-      <c r="A11" s="1" t="n">
+    <row r="11" spans="1:6">
+      <c r="A11" s="1">
         <v>9</v>
       </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t xml:space="preserve">            Two races including Some other race</t>
-        </is>
-      </c>
-      <c r="C11" t="n">
+      <c r="B11" t="s">
+        <v>14</v>
+      </c>
+      <c r="C11">
         <v>405</v>
       </c>
-      <c r="D11" t="n">
+      <c r="D11">
         <v>1236</v>
       </c>
-      <c r="E11" t="n">
+      <c r="E11">
         <v>144</v>
       </c>
-      <c r="F11" t="n">
+      <c r="F11">
         <v>471</v>
       </c>
     </row>
-    <row r="12">
-      <c r="A12" s="1" t="n">
+    <row r="12" spans="1:6">
+      <c r="A12" s="1">
         <v>10</v>
       </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t xml:space="preserve">            Two races excluding Some other race, and three or more races</t>
-        </is>
-      </c>
-      <c r="C12" t="n">
+      <c r="B12" t="s">
+        <v>15</v>
+      </c>
+      <c r="C12">
         <v>7261</v>
       </c>
-      <c r="D12" t="n">
+      <c r="D12">
         <v>10650</v>
       </c>
-      <c r="E12" t="n">
+      <c r="E12">
         <v>10371</v>
       </c>
-      <c r="F12" t="n">
+      <c r="F12">
         <v>11064</v>
       </c>
     </row>
-    <row r="13">
-      <c r="A13" s="1" t="n">
+    <row r="13" spans="1:6">
+      <c r="A13" s="1">
         <v>11</v>
       </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t xml:space="preserve">    Hispanic or Latino:</t>
-        </is>
-      </c>
-      <c r="C13" t="n">
+      <c r="B13" t="s">
+        <v>16</v>
+      </c>
+      <c r="C13">
         <v>18653</v>
       </c>
-      <c r="D13" t="n">
+      <c r="D13">
         <v>23098</v>
       </c>
-      <c r="E13" t="n">
+      <c r="E13">
         <v>20878</v>
       </c>
-      <c r="F13" t="n">
+      <c r="F13">
         <v>22979</v>
       </c>
     </row>
-    <row r="14">
-      <c r="A14" s="1" t="n">
+    <row r="14" spans="1:6">
+      <c r="A14" s="1">
         <v>12</v>
       </c>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t xml:space="preserve">        White alone</t>
-        </is>
-      </c>
-      <c r="C14" t="n">
+      <c r="B14" t="s">
+        <v>17</v>
+      </c>
+      <c r="C14">
         <v>12155</v>
       </c>
-      <c r="D14" t="n">
+      <c r="D14">
         <v>12815</v>
       </c>
-      <c r="E14" t="n">
+      <c r="E14">
         <v>11119</v>
       </c>
-      <c r="F14" t="n">
+      <c r="F14">
         <v>14285</v>
       </c>
     </row>
-    <row r="15">
-      <c r="A15" s="1" t="n">
+    <row r="15" spans="1:6">
+      <c r="A15" s="1">
         <v>13</v>
       </c>
-      <c r="B15" t="inlineStr">
-        <is>
-          <t xml:space="preserve">        Black or African American alone</t>
-        </is>
-      </c>
-      <c r="C15" t="n">
+      <c r="B15" t="s">
+        <v>18</v>
+      </c>
+      <c r="C15">
         <v>1440</v>
       </c>
-      <c r="D15" t="n">
+      <c r="D15">
         <v>2612</v>
       </c>
-      <c r="E15" t="n">
+      <c r="E15">
         <v>3332</v>
       </c>
-      <c r="F15" t="n">
+      <c r="F15">
         <v>1277</v>
       </c>
     </row>
-    <row r="16">
-      <c r="A16" s="1" t="n">
+    <row r="16" spans="1:6">
+      <c r="A16" s="1">
         <v>14</v>
       </c>
-      <c r="B16" t="inlineStr">
-        <is>
-          <t xml:space="preserve">        American Indian and Alaska Native alone</t>
-        </is>
-      </c>
-      <c r="C16" t="n">
+      <c r="B16" t="s">
+        <v>19</v>
+      </c>
+      <c r="C16">
         <v>651</v>
       </c>
-      <c r="D16" t="n">
+      <c r="D16">
         <v>1944</v>
       </c>
-      <c r="E16" t="n">
+      <c r="E16">
         <v>330</v>
       </c>
-      <c r="F16" t="n">
+      <c r="F16">
         <v>323</v>
       </c>
     </row>
-    <row r="17">
-      <c r="A17" s="1" t="n">
+    <row r="17" spans="1:6">
+      <c r="A17" s="1">
         <v>15</v>
       </c>
-      <c r="B17" t="inlineStr">
-        <is>
-          <t xml:space="preserve">        Asian alone</t>
-        </is>
-      </c>
-      <c r="C17" t="n">
+      <c r="B17" t="s">
+        <v>20</v>
+      </c>
+      <c r="C17">
         <v>81</v>
       </c>
-      <c r="D17" t="n">
+      <c r="D17">
         <v>197</v>
       </c>
-      <c r="E17" t="n">
+      <c r="E17">
         <v>0</v>
       </c>
-      <c r="F17" t="n">
+      <c r="F17">
         <v>144</v>
       </c>
     </row>
-    <row r="18">
-      <c r="A18" s="1" t="n">
+    <row r="18" spans="1:6">
+      <c r="A18" s="1">
         <v>16</v>
       </c>
-      <c r="B18" t="inlineStr">
-        <is>
-          <t xml:space="preserve">        Native Hawaiian and Other Pacific Islander alone</t>
-        </is>
-      </c>
-      <c r="C18" t="n">
+      <c r="B18" t="s">
+        <v>21</v>
+      </c>
+      <c r="C18">
         <v>316</v>
       </c>
-      <c r="D18" t="n">
+      <c r="D18">
         <v>39</v>
       </c>
-      <c r="E18" t="n">
+      <c r="E18">
         <v>0</v>
       </c>
-      <c r="F18" t="n">
+      <c r="F18">
         <v>0</v>
       </c>
     </row>
-    <row r="19">
-      <c r="A19" s="1" t="n">
+    <row r="19" spans="1:6">
+      <c r="A19" s="1">
         <v>17</v>
       </c>
-      <c r="B19" t="inlineStr">
-        <is>
-          <t xml:space="preserve">        Some other race alone</t>
-        </is>
-      </c>
-      <c r="C19" t="n">
+      <c r="B19" t="s">
+        <v>22</v>
+      </c>
+      <c r="C19">
         <v>2282</v>
       </c>
-      <c r="D19" t="n">
+      <c r="D19">
         <v>3482</v>
       </c>
-      <c r="E19" t="n">
+      <c r="E19">
         <v>4409</v>
       </c>
-      <c r="F19" t="n">
+      <c r="F19">
         <v>5214</v>
       </c>
     </row>
-    <row r="20">
-      <c r="A20" s="1" t="n">
+    <row r="20" spans="1:6">
+      <c r="A20" s="1">
         <v>18</v>
       </c>
-      <c r="B20" t="inlineStr">
-        <is>
-          <t xml:space="preserve">        Two or more races:</t>
-        </is>
-      </c>
-      <c r="C20" t="n">
+      <c r="B20" t="s">
+        <v>23</v>
+      </c>
+      <c r="C20">
         <v>1728</v>
       </c>
-      <c r="D20" t="n">
+      <c r="D20">
         <v>2009</v>
       </c>
-      <c r="E20" t="n">
+      <c r="E20">
         <v>1688</v>
       </c>
-      <c r="F20" t="n">
+      <c r="F20">
         <v>1736</v>
       </c>
     </row>
-    <row r="21">
-      <c r="A21" s="1" t="n">
+    <row r="21" spans="1:6">
+      <c r="A21" s="1">
         <v>19</v>
       </c>
-      <c r="B21" t="inlineStr">
-        <is>
-          <t xml:space="preserve">            Two races including Some other race</t>
-        </is>
-      </c>
-      <c r="C21" t="n">
+      <c r="B21" t="s">
+        <v>24</v>
+      </c>
+      <c r="C21">
         <v>529</v>
       </c>
-      <c r="D21" t="n">
+      <c r="D21">
         <v>578</v>
       </c>
-      <c r="E21" t="n">
+      <c r="E21">
         <v>766</v>
       </c>
-      <c r="F21" t="n">
+      <c r="F21">
         <v>571</v>
       </c>
     </row>
-    <row r="22">
-      <c r="A22" s="1" t="n">
+    <row r="22" spans="1:6">
+      <c r="A22" s="1">
         <v>20</v>
       </c>
-      <c r="B22" t="inlineStr">
-        <is>
-          <t xml:space="preserve">            Two races excluding Some other race, and three or more races</t>
-        </is>
-      </c>
-      <c r="C22" t="n">
+      <c r="B22" t="s">
+        <v>25</v>
+      </c>
+      <c r="C22">
         <v>1199</v>
       </c>
-      <c r="D22" t="n">
+      <c r="D22">
         <v>1431</v>
       </c>
-      <c r="E22" t="n">
+      <c r="E22">
         <v>922</v>
       </c>
-      <c r="F22" t="n">
+      <c r="F22">
         <v>1165</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>